<commit_message>
make sure all code is up to date. Including transcripts from each algorithms run and data on each
</commit_message>
<xml_diff>
--- a/hw01/Algorithm_Data.xlsx
+++ b/hw01/Algorithm_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25540" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
   <dimension ref="A3:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>